<commit_message>
still shit, hope i know how to solve
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
   <si>
     <t>Bank Name</t>
   </si>
@@ -23,15 +23,6 @@
   </si>
   <si>
     <t>Operation</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Balance</t>
   </si>
   <si>
     <t>Total</t>
@@ -419,13 +410,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,253 +426,160 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>-20</v>
       </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>2018</v>
-      </c>
-      <c r="G2">
-        <v>588</v>
-      </c>
-      <c r="H2">
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>-10</v>
       </c>
-      <c r="E3">
-        <v>11</v>
-      </c>
-      <c r="F3">
-        <v>2018</v>
-      </c>
-      <c r="G3">
-        <v>450</v>
-      </c>
-      <c r="H3">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>-10</v>
       </c>
-      <c r="E4">
-        <v>12</v>
-      </c>
-      <c r="F4">
-        <v>2018</v>
-      </c>
-      <c r="G4">
-        <v>578</v>
-      </c>
-      <c r="H4">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>100</v>
       </c>
-      <c r="E5">
-        <v>12</v>
-      </c>
-      <c r="F5">
-        <v>2018</v>
-      </c>
-      <c r="G5">
-        <v>870</v>
-      </c>
-      <c r="H5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>-30</v>
       </c>
-      <c r="E6">
-        <v>12</v>
-      </c>
-      <c r="F6">
-        <v>2018</v>
-      </c>
-      <c r="G6">
-        <v>548</v>
-      </c>
-      <c r="H6">
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>500</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>2019</v>
-      </c>
-      <c r="G7">
-        <v>700</v>
-      </c>
-      <c r="H7">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12">
-        <v>2568</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>-40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
almost done, need to fix up date and currency columns
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
   <si>
     <t>Bank Name</t>
   </si>
@@ -25,15 +25,24 @@
     <t>Operation</t>
   </si>
   <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Сurrency</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
     <t>Total</t>
   </si>
   <si>
-    <t>('SuperBank', 6623)</t>
-  </si>
-  <si>
-    <t>('SuperBank', 6678)</t>
-  </si>
-  <si>
     <t>SuperBank</t>
   </si>
   <si>
@@ -43,22 +52,25 @@
     <t>6678</t>
   </si>
   <si>
+    <t>6623</t>
+  </si>
+  <si>
     <t>1238</t>
   </si>
   <si>
-    <t>6623</t>
-  </si>
-  <si>
     <t>1253</t>
   </si>
   <si>
-    <t>nan</t>
+    <t>EUR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -111,11 +123,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,13 +423,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,159 +439,314 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>6678</v>
       </c>
       <c r="D2">
         <v>-20</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>588</v>
+      </c>
+      <c r="F2" s="2">
+        <v>43375.62273148148</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>2018</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>1238</v>
       </c>
       <c r="D3">
         <v>-10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>450</v>
+      </c>
+      <c r="F3" s="2">
+        <v>43409.44231481481</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3">
+        <v>2018</v>
+      </c>
+      <c r="I3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>6678</v>
       </c>
       <c r="D4">
         <v>-10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>578</v>
+      </c>
+      <c r="F4" s="2">
+        <v>43436.62273148148</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>2018</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>6623</v>
       </c>
       <c r="D5">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>870</v>
+      </c>
+      <c r="F5" s="2">
+        <v>43437.41219907408</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>2018</v>
+      </c>
+      <c r="I5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>6678</v>
       </c>
       <c r="D6">
         <v>-30</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>548</v>
+      </c>
+      <c r="F6" s="2">
+        <v>43438.62273148148</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>2018</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>1253</v>
       </c>
       <c r="D7">
         <v>500</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>700</v>
+      </c>
+      <c r="F7" s="2">
+        <v>43467.75717592592</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>2019</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>548</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9">
+        <v>870</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
       <c r="C10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <v>450</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>700</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>2568</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>6623</v>
       </c>
       <c r="D13">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>6678</v>
       </c>
       <c r="D14">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>6678</v>
+      </c>
+      <c r="D15">
         <v>-40</v>
       </c>
     </row>

</xml_diff>